<commit_message>
fix to upload function
</commit_message>
<xml_diff>
--- a/app/static/uploads/partner.xlsx
+++ b/app/static/uploads/partner.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danilo/Documents/bapco/webtools settings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dp/py3/webtools/app/static/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68C27AEA-ECD2-AE40-9542-93BA1A213F22}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="6460" windowWidth="27240" windowHeight="16440" xr2:uid="{87856FE3-253F-CB44-BEE0-3E4FCC7366C9}"/>
+    <workbookView xWindow="1560" yWindow="1480" windowWidth="27240" windowHeight="16440" xr2:uid="{87856FE3-253F-CB44-BEE0-3E4FCC7366C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Partner</t>
   </si>
@@ -49,6 +48,12 @@
   </si>
   <si>
     <t>Directorate</t>
+  </si>
+  <si>
+    <t>QSR</t>
+  </si>
+  <si>
+    <t>Quasar</t>
   </si>
 </sst>
 </file>
@@ -409,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD97D0E0-CDF0-2941-818E-9CDA5D7B67C3}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,6 +465,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>